<commit_message>
Update for 5.0.0 (#49)
* Update for 5.0.0

* Small cleanup

* Update workflow

* More updates

* Cleanup readme

* Small tweak
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -105,16 +105,16 @@
     <t>HasFlag (ns)</t>
   </si>
   <si>
-    <t>System.Enum (.NET 5.0)</t>
-  </si>
-  <si>
-    <t>Enums.NET (.NET 5.0)</t>
-  </si>
-  <si>
     <t>System.Enum (.NET Framework 4.8)</t>
   </si>
   <si>
     <t>Enums.NET (.NET Framework 4.8)</t>
+  </si>
+  <si>
+    <t>System.Enum (.NET 8.0)</t>
+  </si>
+  <si>
+    <t>Enums.NET (.NET 8.0)</t>
   </si>
 </sst>
 </file>
@@ -197,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -208,9 +208,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -269,7 +268,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>System.Enum (.NET 5.0)</c:v>
+                  <c:v>System.Enum (.NET 8.0)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -308,19 +307,19 @@
             <c:numRef>
               <c:f>Sheet2!$B$2:$E$2</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>229.86</c:v>
+                  <c:v>172.52</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>224.62</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="#,##0.00">
-                  <c:v>1011.5</c:v>
+                  <c:v>66.28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>132.62299999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>192</c:v>
+                  <c:v>169.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -335,7 +334,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Enums.NET (.NET 5.0)</c:v>
+                  <c:v>Enums.NET (.NET 8.0)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -374,19 +373,19 @@
             <c:numRef>
               <c:f>Sheet2!$B$3:$E$3</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>73.16</c:v>
+                  <c:v>71.510000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.39</c:v>
+                  <c:v>11.48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.06</c:v>
+                  <c:v>5.81</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>239</c:v>
+                  <c:v>206.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -440,19 +439,19 @@
             <c:numRef>
               <c:f>Sheet2!$B$4:$E$4</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>809.14</c:v>
+                <c:pt idx="0">
+                  <c:v>807.94</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6800.69</c:v>
+                  <c:v>8599.8209999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1661.08</c:v>
+                  <c:v>1760.3030000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5154.6000000000004</c:v>
+                  <c:v>5250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -506,19 +505,19 @@
             <c:numRef>
               <c:f>Sheet2!$B$5:$E$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>136.46</c:v>
+                  <c:v>131.11000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.04</c:v>
+                  <c:v>20.03</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.89</c:v>
+                  <c:v>16.846</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>244.5</c:v>
+                  <c:v>244.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -534,12 +533,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="234639360"/>
-        <c:axId val="145334272"/>
+        <c:axId val="153624576"/>
+        <c:axId val="153158784"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="234639360"/>
+        <c:axId val="153624576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -548,7 +547,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145334272"/>
+        <c:crossAx val="153158784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -556,18 +555,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145334272"/>
+        <c:axId val="153158784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="234639360"/>
+        <c:crossAx val="153624576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1037,7 +1036,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,70 +1064,70 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" s="4">
-        <v>229.86</v>
+        <v>172.52</v>
       </c>
       <c r="C2" s="4">
-        <v>224.62</v>
-      </c>
-      <c r="D2" s="6">
-        <v>1011.5</v>
-      </c>
-      <c r="E2">
-        <v>192</v>
+        <v>66.28</v>
+      </c>
+      <c r="D2" s="4">
+        <v>132.62299999999999</v>
+      </c>
+      <c r="E2" s="5">
+        <v>169.9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B3" s="4">
-        <v>73.16</v>
+        <v>71.510000000000005</v>
       </c>
       <c r="C3" s="4">
-        <v>23.39</v>
+        <v>11.48</v>
       </c>
       <c r="D3" s="4">
-        <v>24.06</v>
-      </c>
-      <c r="E3">
-        <v>239</v>
+        <v>5.81</v>
+      </c>
+      <c r="E3" s="5">
+        <v>206.7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4">
-        <v>809.14</v>
+        <v>29</v>
+      </c>
+      <c r="B4" s="5">
+        <v>807.94</v>
       </c>
       <c r="C4" s="5">
-        <v>6800.69</v>
+        <v>8599.8209999999999</v>
       </c>
       <c r="D4" s="5">
-        <v>1661.08</v>
+        <v>1760.3030000000001</v>
       </c>
       <c r="E4" s="5">
-        <v>5154.6000000000004</v>
+        <v>5250</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5">
-        <v>136.46</v>
-      </c>
-      <c r="C5">
-        <v>20.04</v>
-      </c>
-      <c r="D5">
-        <v>16.89</v>
-      </c>
-      <c r="E5">
-        <v>244.5</v>
+        <v>30</v>
+      </c>
+      <c r="B5" s="5">
+        <v>131.11000000000001</v>
+      </c>
+      <c r="C5" s="5">
+        <v>20.03</v>
+      </c>
+      <c r="D5" s="5">
+        <v>16.846</v>
+      </c>
+      <c r="E5" s="5">
+        <v>244.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>